<commit_message>
working version 0.2 buttons are cursor pointers now
</commit_message>
<xml_diff>
--- a/extracter/homychat.xlsx
+++ b/extracter/homychat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
@@ -31,7 +31,7 @@
     <t xml:space="preserve">Название темы:</t>
   </si>
   <si>
-    <t xml:space="preserve">original</t>
+    <t xml:space="preserve">regular_alias_words</t>
   </si>
   <si>
     <t xml:space="preserve">Оригинал</t>
@@ -19015,14 +19015,14 @@
   </sheetPr>
   <dimension ref="A1:B3163"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1203" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1173" activeCellId="0" sqref="A1173"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="37.919028340081"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.9554655870445"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.2429149797571"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.3846153846154"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>

<commit_message>
working version 0.3 load voice added
</commit_message>
<xml_diff>
--- a/extracter/homychat.xlsx
+++ b/extracter/homychat.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="993" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" state="visible" r:id="rId2"/>
@@ -7258,7 +7258,7 @@
     <t xml:space="preserve">оборотень</t>
   </si>
   <si>
-    <t xml:space="preserve">odd number flavour</t>
+    <t xml:space="preserve">odd number</t>
   </si>
   <si>
     <t xml:space="preserve">нечетное число</t>
@@ -19015,14 +19015,14 @@
   </sheetPr>
   <dimension ref="A1:B3163"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B13" activeCellId="0" sqref="B13"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1167" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1210" activeCellId="0" sqref="A1210"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.2429149797571"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="38.5627530364372"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7044534412956"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.57085020242915"/>
   </cols>
   <sheetData>

</xml_diff>